<commit_message>
Too complex to debug in notebook, breaking up into python modules and overlay a pycharm project setup
</commit_message>
<xml_diff>
--- a/UseCase816372.xlsx
+++ b/UseCase816372.xlsx
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AF43" sqref="AF43"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AH15" sqref="AH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -732,7 +732,7 @@
         <v>3</v>
       </c>
       <c r="J2" s="18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2" s="15">
         <v>1</v>
@@ -804,7 +804,7 @@
         <v>4</v>
       </c>
       <c r="J3" s="18">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L3" s="16">
         <v>0</v>
@@ -869,7 +869,7 @@
         <v>5</v>
       </c>
       <c r="J4" s="18">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:30">
@@ -979,7 +979,7 @@
       <c r="R12" s="23"/>
       <c r="S12" s="23">
         <f>(S10*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L14:T14))-((1-LR0)*DISR*MAX(V13:AD13))</f>
-        <v>-21.650921690504589</v>
+        <v>-4.925569138483338</v>
       </c>
       <c r="T12" s="23"/>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="V13" s="25">
         <f>(V11*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V15:AD15))-((1-LR0)*DISR*MAX(L14:T14))</f>
-        <v>16.098332385059081</v>
+        <v>3.3240901237305653</v>
       </c>
       <c r="W13" s="25"/>
       <c r="X13" s="25"/>
@@ -1029,7 +1029,7 @@
       <c r="P14" s="23"/>
       <c r="Q14" s="23">
         <f>(Q12*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L16:T16))-((1-LR0)*DISR*MAX(V15:AD15))</f>
-        <v>-8.9442401251953125</v>
+        <v>-2.133604212539062</v>
       </c>
       <c r="R14" s="23"/>
       <c r="S14" s="23"/>
@@ -1044,7 +1044,7 @@
       <c r="W15" s="25"/>
       <c r="X15" s="25">
         <f>(X13*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V17:AD17))-((1-LR0)*DISR*MAX(L16:T16))</f>
-        <v>7.8406157031249997</v>
+        <v>1.5495981406249999</v>
       </c>
       <c r="Y15" s="25"/>
       <c r="Z15" s="25"/>
@@ -1066,7 +1066,7 @@
       <c r="Q16" s="23"/>
       <c r="R16" s="23">
         <f>(R14*LR0)+((1-LR0)*PLAY)+(0)-((1-LR0)*DISR*MAX(V17:AD17))</f>
-        <v>-3.1225312499999998</v>
+        <v>-0.81450624999999999</v>
       </c>
       <c r="S16" s="23"/>
       <c r="T16" s="23"/>
@@ -1084,7 +1084,7 @@
       <c r="V17" s="25"/>
       <c r="W17" s="25">
         <f>(W15*LR0)+((1-LR0)*DISR*WIN)</f>
-        <v>4.5125000000000002</v>
+        <v>0.90249999999999997</v>
       </c>
       <c r="X17" s="25"/>
       <c r="Y17" s="25"/>
@@ -1129,7 +1129,7 @@
       <c r="R20" s="23"/>
       <c r="S20" s="26">
         <f>S12</f>
-        <v>-21.650921690504589</v>
+        <v>-4.925569138483338</v>
       </c>
       <c r="T20" s="23"/>
     </row>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="V21" s="27">
         <f>V13</f>
-        <v>16.098332385059081</v>
+        <v>3.3240901237305653</v>
       </c>
       <c r="W21" s="25"/>
       <c r="X21" s="25"/>
@@ -1170,12 +1170,12 @@
       <c r="P22" s="23"/>
       <c r="Q22" s="26">
         <f>Q14</f>
-        <v>-8.9442401251953125</v>
+        <v>-2.133604212539062</v>
       </c>
       <c r="R22" s="23"/>
       <c r="S22" s="23">
         <f>(S20*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L24:T24))-((1-LR0)*DISR*MAX(V23:AD23))</f>
-        <v>-14.213612736853728</v>
+        <v>-3.2131003002136755</v>
       </c>
       <c r="T22" s="23"/>
     </row>
@@ -1196,12 +1196,12 @@
       </c>
       <c r="V23" s="25">
         <f>(V21*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V25:AD25))-((1-LR0)*DISR*MAX(L24:T24))</f>
-        <v>12.479758669477562</v>
+        <v>2.4728309724814501</v>
       </c>
       <c r="W23" s="25"/>
       <c r="X23" s="27">
         <f>X15</f>
-        <v>7.8406157031249997</v>
+        <v>1.5495981406249999</v>
       </c>
       <c r="Y23" s="25"/>
       <c r="Z23" s="25"/>
@@ -1227,11 +1227,11 @@
       <c r="P24" s="23"/>
       <c r="Q24" s="23">
         <f>(Q22*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L26:T26))-((1-LR0)*DISR*MAX(V25:AD25))</f>
-        <v>-10.546731251796874</v>
+        <v>-2.4868158659843749</v>
       </c>
       <c r="R24" s="26">
         <f>R16</f>
-        <v>-3.1225312499999998</v>
+        <v>-0.81450624999999999</v>
       </c>
       <c r="S24" s="23"/>
       <c r="T24" s="23"/>
@@ -1244,11 +1244,11 @@
       <c r="V25" s="25"/>
       <c r="W25" s="27">
         <f>W17</f>
-        <v>4.5125000000000002</v>
+        <v>0.90249999999999997</v>
       </c>
       <c r="X25" s="25">
         <f>(X23*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V27:AD27))-((1-LR0)*DISR*MAX(L26:T26))</f>
-        <v>8.7609502460937492</v>
+        <v>1.7413125492187498</v>
       </c>
       <c r="Y25" s="25"/>
       <c r="Z25" s="25"/>
@@ -1270,7 +1270,7 @@
       <c r="Q26" s="23"/>
       <c r="R26" s="23">
         <f>(R24*LR0)+((1-LR0)*PLAY)+(0)-((1-LR0)*DISR*MAX(V27:AD27))</f>
-        <v>-3.4822843750000003</v>
+        <v>-0.89595687499999987</v>
       </c>
       <c r="S26" s="23"/>
       <c r="T26" s="23"/>
@@ -1290,7 +1290,7 @@
       <c r="V27" s="25"/>
       <c r="W27" s="25">
         <f>(W25*LR0)+((1-LR0)*DISR*WIN)</f>
-        <v>4.7381250000000001</v>
+        <v>0.94762499999999994</v>
       </c>
       <c r="X27" s="25"/>
       <c r="Y27" s="25"/>
@@ -1340,7 +1340,7 @@
       <c r="R30" s="23"/>
       <c r="S30" s="26">
         <f>S22</f>
-        <v>-14.213612736853728</v>
+        <v>-3.2131003002136755</v>
       </c>
       <c r="T30" s="23"/>
     </row>
@@ -1351,7 +1351,7 @@
       </c>
       <c r="V31" s="27">
         <f>V23</f>
-        <v>12.479758669477562</v>
+        <v>2.4728309724814501</v>
       </c>
       <c r="W31" s="25"/>
       <c r="X31" s="25"/>
@@ -1383,12 +1383,12 @@
       <c r="P32" s="23"/>
       <c r="Q32" s="26">
         <f>Q24</f>
-        <v>-10.546731251796874</v>
+        <v>-2.4868158659843749</v>
       </c>
       <c r="R32" s="23"/>
       <c r="S32" s="23">
         <f>(S30*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L34:T34))-((1-LR0)*DISR*MAX(V33:AD33))</f>
-        <v>-14.362637973576867</v>
+        <v>-3.2428717286147255</v>
       </c>
       <c r="T32" s="23"/>
     </row>
@@ -1412,12 +1412,12 @@
       </c>
       <c r="V33" s="25">
         <f>(V31*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V35:AD35))-((1-LR0)*DISR*MAX(L34:T34))</f>
-        <v>12.697169737724852</v>
+        <v>2.5192416996305176</v>
       </c>
       <c r="W33" s="25"/>
       <c r="X33" s="27">
         <f>X25</f>
-        <v>8.7609502460937492</v>
+        <v>1.7413125492187498</v>
       </c>
       <c r="Y33" s="25"/>
       <c r="Z33" s="25"/>
@@ -1444,11 +1444,11 @@
       <c r="P34" s="23"/>
       <c r="Q34" s="23">
         <f>(Q32*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L36:T36))-((1-LR0)*DISR*MAX(V35:AD35))</f>
-        <v>-10.725940875239257</v>
+        <v>-2.5254541334853515</v>
       </c>
       <c r="R34" s="26">
         <f>R26</f>
-        <v>-3.4822843750000003</v>
+        <v>-0.89595687499999987</v>
       </c>
       <c r="S34" s="23"/>
       <c r="T34" s="23"/>
@@ -1460,11 +1460,11 @@
       <c r="V35" s="25"/>
       <c r="W35" s="27">
         <f>W27</f>
-        <v>4.7381250000000001</v>
+        <v>0.94762499999999994</v>
       </c>
       <c r="X35" s="25">
         <f>(X33*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V37:AD37))-((1-LR0)*DISR*MAX(L36:T36))</f>
-        <v>8.8425708097656237</v>
+        <v>1.7584477244531249</v>
       </c>
       <c r="Y35" s="25"/>
       <c r="Z35" s="25"/>
@@ -1485,7 +1485,7 @@
       <c r="Q36" s="23"/>
       <c r="R36" s="23">
         <f>(R34*LR0)+((1-LR0)*PLAY)+(0)-((1-LR0)*DISR*MAX(V37:AD37))</f>
-        <v>-3.5104533593749996</v>
+        <v>-0.90206567187499997</v>
       </c>
       <c r="S36" s="23"/>
       <c r="T36" s="23"/>
@@ -1497,7 +1497,7 @@
       <c r="V37" s="25"/>
       <c r="W37" s="25">
         <f>(W35*LR0)+((1-LR0)*DISR*WIN)</f>
-        <v>4.7494062499999998</v>
+        <v>0.94988125000000001</v>
       </c>
       <c r="X37" s="25"/>
       <c r="Y37" s="25"/>
@@ -1520,7 +1520,7 @@
       <c r="R40" s="23"/>
       <c r="S40" s="26">
         <f>S32</f>
-        <v>-14.362637973576867</v>
+        <v>-3.2428717286147255</v>
       </c>
       <c r="T40" s="23"/>
     </row>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="V41" s="27">
         <f>V33</f>
-        <v>12.697169737724852</v>
+        <v>2.5192416996305176</v>
       </c>
       <c r="W41" s="25"/>
       <c r="X41" s="25"/>
@@ -1552,12 +1552,12 @@
       <c r="P42" s="23"/>
       <c r="Q42" s="26">
         <f>Q34</f>
-        <v>-10.725940875239257</v>
+        <v>-2.5254541334853515</v>
       </c>
       <c r="R42" s="23"/>
       <c r="S42" s="23">
         <f>(S40*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L44:T44))-((1-LR0)*DISR*MAX(V43:AD43))</f>
-        <v>-14.433414443013312</v>
+        <v>-3.2580235579014278</v>
       </c>
       <c r="T42" s="23"/>
     </row>
@@ -1567,12 +1567,12 @@
       </c>
       <c r="V43" s="25">
         <f>(V41*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V45:AD45))-((1-LR0)*DISR*MAX(L44:T44))</f>
-        <v>12.739167188364025</v>
+        <v>2.5282722466520822</v>
       </c>
       <c r="W43" s="25"/>
       <c r="X43" s="27">
         <f>X35</f>
-        <v>8.8425708097656237</v>
+        <v>1.7584477244531249</v>
       </c>
       <c r="Y43" s="25"/>
       <c r="Z43" s="25"/>
@@ -1592,11 +1592,11 @@
       <c r="P44" s="23"/>
       <c r="Q44" s="23">
         <f>(Q42*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L46:T46))-((1-LR0)*DISR*MAX(V45:AD45))</f>
-        <v>-10.742336303091308</v>
+        <v>-2.5289504142901365</v>
       </c>
       <c r="R44" s="26">
         <f>R36</f>
-        <v>-3.5104533593749996</v>
+        <v>-0.90206567187499997</v>
       </c>
       <c r="S44" s="23"/>
       <c r="T44" s="23"/>
@@ -1608,11 +1608,11 @@
       <c r="V45" s="25"/>
       <c r="W45" s="27">
         <f>W37</f>
-        <v>4.7494062499999998</v>
+        <v>0.94988125000000001</v>
       </c>
       <c r="X45" s="25">
         <f>(X43*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V47:AD47))-((1-LR0)*DISR*MAX(L46:T46))</f>
-        <v>8.8488914622070318</v>
+        <v>1.759773842441406</v>
       </c>
       <c r="Y45" s="25"/>
       <c r="Z45" s="25"/>
@@ -1633,7 +1633,7 @@
       <c r="Q46" s="23"/>
       <c r="R46" s="23">
         <f>(R44*LR0)+((1-LR0)*PLAY)+(0)-((1-LR0)*DISR*MAX(V47:AD47))</f>
-        <v>-3.5123708750000002</v>
+        <v>-0.90247292499999998</v>
       </c>
       <c r="S46" s="23"/>
       <c r="T46" s="23"/>
@@ -1645,7 +1645,7 @@
       <c r="V47" s="25"/>
       <c r="W47" s="25">
         <f>(W45*LR0)+((1-LR0)*DISR*WIN)</f>
-        <v>4.7499703125000003</v>
+        <v>0.94999406249999996</v>
       </c>
       <c r="X47" s="25"/>
       <c r="Y47" s="25"/>

</xml_diff>

<commit_message>
added new q value routine to assess best-outcome over simple (incorrect) max - bit messy and needs lots of clean up
</commit_message>
<xml_diff>
--- a/UseCase816372.xlsx
+++ b/UseCase816372.xlsx
@@ -110,7 +110,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,14 +123,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -326,7 +321,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -364,7 +359,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -378,11 +372,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,7 +678,7 @@
   <dimension ref="A1:AD47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AH15" sqref="AH15"/>
+      <selection activeCell="W47" sqref="W47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -692,101 +690,101 @@
     <col min="7" max="7" width="6.28515625" customWidth="1"/>
     <col min="8" max="8" width="5.42578125" customWidth="1"/>
     <col min="9" max="9" width="28.85546875" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" style="16" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" customWidth="1"/>
-    <col min="12" max="20" width="6.85546875" style="16" customWidth="1"/>
-    <col min="21" max="21" width="7.42578125" customWidth="1"/>
-    <col min="22" max="30" width="6.85546875" style="16" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" style="15" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="23" customWidth="1"/>
+    <col min="12" max="20" width="6.85546875" style="23" customWidth="1"/>
+    <col min="21" max="21" width="7.42578125" style="23" customWidth="1"/>
+    <col min="22" max="30" width="6.85546875" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" thickBot="1">
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="19" t="s">
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="20"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="24"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="25"/>
     </row>
     <row r="2" spans="1:30">
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="18">
-        <v>0</v>
-      </c>
-      <c r="L2" s="15">
-        <v>1</v>
-      </c>
-      <c r="M2" s="15">
+      <c r="J2" s="17">
+        <v>0</v>
+      </c>
+      <c r="L2" s="27">
+        <v>1</v>
+      </c>
+      <c r="M2" s="27">
         <v>2</v>
       </c>
-      <c r="N2" s="15">
+      <c r="N2" s="27">
         <v>3</v>
       </c>
-      <c r="O2" s="15">
+      <c r="O2" s="27">
         <v>4</v>
       </c>
-      <c r="P2" s="15">
+      <c r="P2" s="27">
         <v>5</v>
       </c>
-      <c r="Q2" s="15">
+      <c r="Q2" s="27">
         <v>6</v>
       </c>
-      <c r="R2" s="15">
+      <c r="R2" s="27">
         <v>7</v>
       </c>
-      <c r="S2" s="15">
+      <c r="S2" s="27">
         <v>8</v>
       </c>
-      <c r="T2" s="15">
+      <c r="T2" s="27">
         <v>9</v>
       </c>
-      <c r="U2" s="14"/>
-      <c r="V2" s="15">
-        <v>1</v>
-      </c>
-      <c r="W2" s="15">
+      <c r="U2" s="26"/>
+      <c r="V2" s="27">
+        <v>1</v>
+      </c>
+      <c r="W2" s="27">
         <v>2</v>
       </c>
-      <c r="X2" s="15">
+      <c r="X2" s="27">
         <v>3</v>
       </c>
-      <c r="Y2" s="15">
+      <c r="Y2" s="27">
         <v>4</v>
       </c>
-      <c r="Z2" s="15">
+      <c r="Z2" s="27">
         <v>5</v>
       </c>
-      <c r="AA2" s="15">
+      <c r="AA2" s="27">
         <v>6</v>
       </c>
-      <c r="AB2" s="15">
+      <c r="AB2" s="27">
         <v>7</v>
       </c>
-      <c r="AC2" s="15">
+      <c r="AC2" s="27">
         <v>8</v>
       </c>
-      <c r="AD2" s="15">
+      <c r="AD2" s="27">
         <v>9</v>
       </c>
     </row>
@@ -800,64 +798,64 @@
       <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="18">
-        <v>1</v>
-      </c>
-      <c r="L3" s="16">
-        <v>0</v>
-      </c>
-      <c r="M3" s="16">
-        <v>0</v>
-      </c>
-      <c r="N3" s="16">
-        <v>0</v>
-      </c>
-      <c r="O3" s="16">
-        <v>0</v>
-      </c>
-      <c r="P3" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="16">
-        <v>0</v>
-      </c>
-      <c r="R3" s="16">
-        <v>0</v>
-      </c>
-      <c r="S3" s="16">
-        <v>0</v>
-      </c>
-      <c r="T3" s="16">
-        <v>0</v>
-      </c>
-      <c r="V3" s="16">
-        <v>0</v>
-      </c>
-      <c r="W3" s="16">
-        <v>0</v>
-      </c>
-      <c r="X3" s="16">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="16">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="16">
+      <c r="J3" s="17">
+        <v>1</v>
+      </c>
+      <c r="L3" s="23">
+        <v>0</v>
+      </c>
+      <c r="M3" s="23">
+        <v>0</v>
+      </c>
+      <c r="N3" s="23">
+        <v>0</v>
+      </c>
+      <c r="O3" s="23">
+        <v>0</v>
+      </c>
+      <c r="P3" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="23">
+        <v>0</v>
+      </c>
+      <c r="R3" s="23">
+        <v>0</v>
+      </c>
+      <c r="S3" s="23">
+        <v>0</v>
+      </c>
+      <c r="T3" s="23">
+        <v>0</v>
+      </c>
+      <c r="V3" s="23">
+        <v>0</v>
+      </c>
+      <c r="W3" s="23">
+        <v>0</v>
+      </c>
+      <c r="X3" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="23">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="23">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="23">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="23">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="23">
         <v>0</v>
       </c>
     </row>
@@ -865,34 +863,33 @@
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
       <c r="E4" s="12"/>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="18">
+      <c r="J4" s="17">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:30">
-      <c r="I5" s="17"/>
-      <c r="J5" s="18"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="17"/>
     </row>
     <row r="6" spans="1:30" ht="15.75" thickBot="1">
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J6" s="17">
         <v>0.05</v>
       </c>
-      <c r="K6" s="16"/>
     </row>
     <row r="7" spans="1:30">
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
-      <c r="I7" s="17" t="s">
+      <c r="I7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="18">
+      <c r="J7" s="17">
         <v>0.1</v>
       </c>
     </row>
@@ -906,11 +903,11 @@
       <c r="G8" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="18">
-        <v>0.95</v>
+      <c r="J8" s="17">
+        <v>0.8</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="15.75" thickBot="1">
@@ -926,36 +923,36 @@
       <c r="I10" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="K10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
-      <c r="S10" s="23"/>
-      <c r="T10" s="23"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="22"/>
     </row>
     <row r="11" spans="1:30" ht="15.75" thickBot="1">
       <c r="A11" s="2"/>
-      <c r="I11" s="17" t="s">
+      <c r="I11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="U11" s="24" t="s">
+      <c r="U11" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="V11" s="25"/>
-      <c r="W11" s="25"/>
-      <c r="X11" s="25"/>
-      <c r="Y11" s="25"/>
-      <c r="Z11" s="25"/>
-      <c r="AA11" s="25"/>
-      <c r="AB11" s="25"/>
-      <c r="AC11" s="25"/>
-      <c r="AD11" s="25"/>
+      <c r="V11" s="28"/>
+      <c r="W11" s="28"/>
+      <c r="X11" s="28"/>
+      <c r="Y11" s="28"/>
+      <c r="Z11" s="28"/>
+      <c r="AA11" s="28"/>
+      <c r="AB11" s="28"/>
+      <c r="AC11" s="28"/>
+      <c r="AD11" s="28"/>
     </row>
     <row r="12" spans="1:30">
       <c r="A12" s="2"/>
@@ -964,24 +961,24 @@
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
-      <c r="I12" s="17" t="s">
+      <c r="I12" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="K12" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
-      <c r="S12" s="23">
-        <f>(S10*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L14:T14))-((1-LR0)*DISR*MAX(V13:AD13))</f>
-        <v>-4.925569138483338</v>
-      </c>
-      <c r="T12" s="23"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22">
+        <f>(S10*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V13:AD13))</f>
+        <v>-0.19269992857600002</v>
+      </c>
+      <c r="T12" s="22"/>
     </row>
     <row r="13" spans="1:30">
       <c r="A13" s="2">
@@ -993,24 +990,24 @@
       <c r="G13" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="I13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="U13" s="24" t="s">
+      <c r="U13" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="V13" s="25">
-        <f>(V11*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V15:AD15))-((1-LR0)*DISR*MAX(L14:T14))</f>
-        <v>3.3240901237305653</v>
-      </c>
-      <c r="W13" s="25"/>
-      <c r="X13" s="25"/>
-      <c r="Y13" s="25"/>
-      <c r="Z13" s="25"/>
-      <c r="AA13" s="25"/>
-      <c r="AB13" s="25"/>
-      <c r="AC13" s="25"/>
-      <c r="AD13" s="25"/>
+      <c r="V13" s="28">
+        <f>(V11*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L14:T14))</f>
+        <v>0.25355253760000002</v>
+      </c>
+      <c r="W13" s="28"/>
+      <c r="X13" s="28"/>
+      <c r="Y13" s="28"/>
+      <c r="Z13" s="28"/>
+      <c r="AA13" s="28"/>
+      <c r="AB13" s="28"/>
+      <c r="AC13" s="28"/>
+      <c r="AD13" s="28"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" thickBot="1">
       <c r="A14" s="2"/>
@@ -1019,57 +1016,57 @@
         <v>0</v>
       </c>
       <c r="E14" s="12"/>
-      <c r="K14" s="13" t="s">
+      <c r="K14" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23">
-        <f>(Q12*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L16:T16))-((1-LR0)*DISR*MAX(V15:AD15))</f>
-        <v>-2.133604212539062</v>
-      </c>
-      <c r="R14" s="23"/>
-      <c r="S14" s="23"/>
-      <c r="T14" s="23"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22">
+        <f>(Q12*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V15:AD15))</f>
+        <v>-0.33362176000000004</v>
+      </c>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
     </row>
     <row r="15" spans="1:30">
       <c r="A15" s="2"/>
-      <c r="U15" s="24" t="s">
+      <c r="U15" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="V15" s="25"/>
-      <c r="W15" s="25"/>
-      <c r="X15" s="25">
-        <f>(X13*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V17:AD17))-((1-LR0)*DISR*MAX(L16:T16))</f>
-        <v>1.5495981406249999</v>
-      </c>
-      <c r="Y15" s="25"/>
-      <c r="Z15" s="25"/>
-      <c r="AA15" s="25"/>
-      <c r="AB15" s="25"/>
-      <c r="AC15" s="25"/>
-      <c r="AD15" s="25"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="28">
+        <f>(X13*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L16:T16))</f>
+        <v>0.43897600000000003</v>
+      </c>
+      <c r="Y15" s="28"/>
+      <c r="Z15" s="28"/>
+      <c r="AA15" s="28"/>
+      <c r="AB15" s="28"/>
+      <c r="AC15" s="28"/>
+      <c r="AD15" s="28"/>
     </row>
     <row r="16" spans="1:30" ht="15.75" thickBot="1">
       <c r="A16" s="2"/>
-      <c r="K16" s="13" t="s">
+      <c r="K16" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23">
-        <f>(R14*LR0)+((1-LR0)*PLAY)+(0)-((1-LR0)*DISR*MAX(V17:AD17))</f>
-        <v>-0.81450624999999999</v>
-      </c>
-      <c r="S16" s="23"/>
-      <c r="T16" s="23"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22">
+        <f>(R14*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V17:AD17))</f>
+        <v>-0.5776</v>
+      </c>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
     </row>
     <row r="17" spans="1:30">
       <c r="A17" s="2"/>
@@ -1078,21 +1075,21 @@
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
-      <c r="U17" s="24" t="s">
+      <c r="U17" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="V17" s="25"/>
-      <c r="W17" s="25">
+      <c r="V17" s="28"/>
+      <c r="W17" s="28">
         <f>(W15*LR0)+((1-LR0)*DISR*WIN)</f>
-        <v>0.90249999999999997</v>
-      </c>
-      <c r="X17" s="25"/>
-      <c r="Y17" s="25"/>
-      <c r="Z17" s="25"/>
-      <c r="AA17" s="25"/>
-      <c r="AB17" s="25"/>
-      <c r="AC17" s="25"/>
-      <c r="AD17" s="25"/>
+        <v>0.76</v>
+      </c>
+      <c r="X17" s="28"/>
+      <c r="Y17" s="28"/>
+      <c r="Z17" s="28"/>
+      <c r="AA17" s="28"/>
+      <c r="AB17" s="28"/>
+      <c r="AC17" s="28"/>
+      <c r="AD17" s="28"/>
     </row>
     <row r="18" spans="1:30">
       <c r="A18" s="2">
@@ -1117,39 +1114,33 @@
     </row>
     <row r="20" spans="1:30">
       <c r="A20" s="2"/>
-      <c r="K20" s="13" t="s">
+      <c r="K20" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
-      <c r="N20" s="23"/>
-      <c r="O20" s="23"/>
-      <c r="P20" s="23"/>
-      <c r="Q20" s="23"/>
-      <c r="R20" s="23"/>
-      <c r="S20" s="26">
-        <f>S12</f>
-        <v>-4.925569138483338</v>
-      </c>
-      <c r="T20" s="23"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="22"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="22"/>
+      <c r="S20" s="22"/>
+      <c r="T20" s="22"/>
     </row>
     <row r="21" spans="1:30" ht="15.75" thickBot="1">
       <c r="A21" s="2"/>
-      <c r="U21" s="24" t="s">
+      <c r="U21" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="V21" s="27">
-        <f>V13</f>
-        <v>3.3240901237305653</v>
-      </c>
-      <c r="W21" s="25"/>
-      <c r="X21" s="25"/>
-      <c r="Y21" s="25"/>
-      <c r="Z21" s="25"/>
-      <c r="AA21" s="25"/>
-      <c r="AB21" s="25"/>
-      <c r="AC21" s="25"/>
-      <c r="AD21" s="25"/>
+      <c r="V21" s="28"/>
+      <c r="W21" s="28"/>
+      <c r="X21" s="28"/>
+      <c r="Y21" s="28"/>
+      <c r="Z21" s="28"/>
+      <c r="AA21" s="28"/>
+      <c r="AB21" s="28"/>
+      <c r="AC21" s="28"/>
+      <c r="AD21" s="28"/>
     </row>
     <row r="22" spans="1:30">
       <c r="A22" s="2"/>
@@ -1160,24 +1151,21 @@
       <c r="E22" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K22" s="13" t="s">
+      <c r="K22" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="26">
-        <f>Q14</f>
-        <v>-2.133604212539062</v>
-      </c>
-      <c r="R22" s="23"/>
-      <c r="S22" s="23">
-        <f>(S20*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L24:T24))-((1-LR0)*DISR*MAX(V23:AD23))</f>
-        <v>-3.2131003002136755</v>
-      </c>
-      <c r="T22" s="23"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="22">
+        <f>(S12*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V23:AD23))</f>
+        <v>-0.25050990714880006</v>
+      </c>
+      <c r="T22" s="22"/>
     </row>
     <row r="23" spans="1:30">
       <c r="A23" s="2">
@@ -1191,24 +1179,21 @@
       <c r="G23" t="s">
         <v>21</v>
       </c>
-      <c r="U23" s="24" t="s">
+      <c r="U23" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="V23" s="25">
-        <f>(V21*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V25:AD25))-((1-LR0)*DISR*MAX(L24:T24))</f>
-        <v>2.4728309724814501</v>
-      </c>
-      <c r="W23" s="25"/>
-      <c r="X23" s="27">
-        <f>X15</f>
-        <v>1.5495981406249999</v>
-      </c>
-      <c r="Y23" s="25"/>
-      <c r="Z23" s="25"/>
-      <c r="AA23" s="25"/>
-      <c r="AB23" s="25"/>
-      <c r="AC23" s="25"/>
-      <c r="AD23" s="25"/>
+      <c r="V23" s="28">
+        <f>(V13*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L24:T24))</f>
+        <v>0.31694067200000003</v>
+      </c>
+      <c r="W23" s="28"/>
+      <c r="X23" s="28"/>
+      <c r="Y23" s="28"/>
+      <c r="Z23" s="28"/>
+      <c r="AA23" s="28"/>
+      <c r="AB23" s="28"/>
+      <c r="AC23" s="28"/>
+      <c r="AD23" s="28"/>
     </row>
     <row r="24" spans="1:30" ht="15.75" thickBot="1">
       <c r="A24" s="2"/>
@@ -1217,63 +1202,57 @@
         <v>0</v>
       </c>
       <c r="E24" s="12"/>
-      <c r="K24" s="13" t="s">
+      <c r="K24" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="L24" s="23"/>
-      <c r="M24" s="23"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23">
-        <f>(Q22*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L26:T26))-((1-LR0)*DISR*MAX(V25:AD25))</f>
-        <v>-2.4868158659843749</v>
-      </c>
-      <c r="R24" s="26">
-        <f>R16</f>
-        <v>-0.81450624999999999</v>
-      </c>
-      <c r="S24" s="23"/>
-      <c r="T24" s="23"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22">
+        <f>(Q14*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V25:AD25))</f>
+        <v>-0.40034611200000003</v>
+      </c>
+      <c r="R24" s="22"/>
+      <c r="S24" s="22"/>
+      <c r="T24" s="22"/>
     </row>
     <row r="25" spans="1:30">
       <c r="A25" s="2"/>
-      <c r="U25" s="24" t="s">
+      <c r="U25" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="V25" s="25"/>
-      <c r="W25" s="27">
-        <f>W17</f>
-        <v>0.90249999999999997</v>
-      </c>
-      <c r="X25" s="25">
-        <f>(X23*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V27:AD27))-((1-LR0)*DISR*MAX(L26:T26))</f>
-        <v>1.7413125492187498</v>
-      </c>
-      <c r="Y25" s="25"/>
-      <c r="Z25" s="25"/>
-      <c r="AA25" s="25"/>
-      <c r="AB25" s="25"/>
-      <c r="AC25" s="25"/>
-      <c r="AD25" s="25"/>
+      <c r="V25" s="28"/>
+      <c r="W25" s="28"/>
+      <c r="X25" s="28">
+        <f>(X15*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L26:T26))</f>
+        <v>0.5048224</v>
+      </c>
+      <c r="Y25" s="28"/>
+      <c r="Z25" s="28"/>
+      <c r="AA25" s="28"/>
+      <c r="AB25" s="28"/>
+      <c r="AC25" s="28"/>
+      <c r="AD25" s="28"/>
     </row>
     <row r="26" spans="1:30" ht="15.75" thickBot="1">
       <c r="A26" s="2"/>
-      <c r="K26" s="13" t="s">
+      <c r="K26" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23">
-        <f>(R24*LR0)+((1-LR0)*PLAY)+(0)-((1-LR0)*DISR*MAX(V27:AD27))</f>
-        <v>-0.89595687499999987</v>
-      </c>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22">
+        <f>(R16*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V27:AD27))</f>
+        <v>-0.63536000000000004</v>
+      </c>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22"/>
     </row>
     <row r="27" spans="1:30">
       <c r="A27" s="2"/>
@@ -1284,21 +1263,21 @@
       <c r="E27" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="U27" s="24" t="s">
+      <c r="U27" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="V27" s="25"/>
-      <c r="W27" s="25">
-        <f>(W25*LR0)+((1-LR0)*DISR*WIN)</f>
-        <v>0.94762499999999994</v>
-      </c>
-      <c r="X27" s="25"/>
-      <c r="Y27" s="25"/>
-      <c r="Z27" s="25"/>
-      <c r="AA27" s="25"/>
-      <c r="AB27" s="25"/>
-      <c r="AC27" s="25"/>
-      <c r="AD27" s="25"/>
+      <c r="V27" s="28"/>
+      <c r="W27" s="28">
+        <f>(W17*LR0)+((1-LR0)*DISR*WIN)</f>
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="X27" s="28"/>
+      <c r="Y27" s="28"/>
+      <c r="Z27" s="28"/>
+      <c r="AA27" s="28"/>
+      <c r="AB27" s="28"/>
+      <c r="AC27" s="28"/>
+      <c r="AD27" s="28"/>
     </row>
     <row r="28" spans="1:30">
       <c r="A28" s="2">
@@ -1309,7 +1288,7 @@
       <c r="E28" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="21" t="s">
         <v>14</v>
       </c>
       <c r="H28" t="s">
@@ -1328,39 +1307,33 @@
     </row>
     <row r="30" spans="1:30">
       <c r="A30" s="2"/>
-      <c r="K30" s="13" t="s">
+      <c r="K30" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="23"/>
-      <c r="P30" s="23"/>
-      <c r="Q30" s="23"/>
-      <c r="R30" s="23"/>
-      <c r="S30" s="26">
-        <f>S22</f>
-        <v>-3.2131003002136755</v>
-      </c>
-      <c r="T30" s="23"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="22"/>
+      <c r="N30" s="22"/>
+      <c r="O30" s="22"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="22"/>
+      <c r="R30" s="22"/>
+      <c r="S30" s="22"/>
+      <c r="T30" s="22"/>
     </row>
     <row r="31" spans="1:30" ht="15.75" thickBot="1">
       <c r="A31" s="2"/>
-      <c r="U31" s="24" t="s">
+      <c r="U31" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="V31" s="27">
-        <f>V23</f>
-        <v>2.4728309724814501</v>
-      </c>
-      <c r="W31" s="25"/>
-      <c r="X31" s="25"/>
-      <c r="Y31" s="25"/>
-      <c r="Z31" s="25"/>
-      <c r="AA31" s="25"/>
-      <c r="AB31" s="25"/>
-      <c r="AC31" s="25"/>
-      <c r="AD31" s="25"/>
+      <c r="V31" s="28"/>
+      <c r="W31" s="28"/>
+      <c r="X31" s="28"/>
+      <c r="Y31" s="28"/>
+      <c r="Z31" s="28"/>
+      <c r="AA31" s="28"/>
+      <c r="AB31" s="28"/>
+      <c r="AC31" s="28"/>
+      <c r="AD31" s="28"/>
     </row>
     <row r="32" spans="1:30">
       <c r="A32" s="2"/>
@@ -1373,24 +1346,21 @@
       <c r="E32" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="K32" s="13" t="s">
+      <c r="K32" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="26">
-        <f>Q24</f>
-        <v>-2.4868158659843749</v>
-      </c>
-      <c r="R32" s="23"/>
-      <c r="S32" s="23">
-        <f>(S30*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L34:T34))-((1-LR0)*DISR*MAX(V33:AD33))</f>
-        <v>-3.2428717286147255</v>
-      </c>
-      <c r="T32" s="23"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="22">
+        <f>(S22*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V33:AD33))</f>
+        <v>-0.26062665339904006</v>
+      </c>
+      <c r="T32" s="22"/>
     </row>
     <row r="33" spans="1:30">
       <c r="A33" s="2">
@@ -1407,24 +1377,21 @@
       <c r="H33" t="s">
         <v>4</v>
       </c>
-      <c r="U33" s="24" t="s">
+      <c r="U33" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="V33" s="25">
-        <f>(V31*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V35:AD35))-((1-LR0)*DISR*MAX(L34:T34))</f>
-        <v>2.5192416996305176</v>
-      </c>
-      <c r="W33" s="25"/>
-      <c r="X33" s="27">
-        <f>X25</f>
-        <v>1.7413125492187498</v>
-      </c>
-      <c r="Y33" s="25"/>
-      <c r="Z33" s="25"/>
-      <c r="AA33" s="25"/>
-      <c r="AB33" s="25"/>
-      <c r="AC33" s="25"/>
-      <c r="AD33" s="25"/>
+      <c r="V33" s="28">
+        <f>(V23*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L34:T34))</f>
+        <v>0.32644889216000006</v>
+      </c>
+      <c r="W33" s="28"/>
+      <c r="X33" s="28"/>
+      <c r="Y33" s="28"/>
+      <c r="Z33" s="28"/>
+      <c r="AA33" s="28"/>
+      <c r="AB33" s="28"/>
+      <c r="AC33" s="28"/>
+      <c r="AD33" s="28"/>
     </row>
     <row r="34" spans="1:30" ht="15.75" thickBot="1">
       <c r="C34" s="10" t="s">
@@ -1434,226 +1401,202 @@
         <v>0</v>
       </c>
       <c r="E34" s="12"/>
-      <c r="K34" s="13" t="s">
+      <c r="K34" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="L34" s="23"/>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="23"/>
-      <c r="P34" s="23"/>
-      <c r="Q34" s="23">
-        <f>(Q32*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L36:T36))-((1-LR0)*DISR*MAX(V35:AD35))</f>
-        <v>-2.5254541334853515</v>
-      </c>
-      <c r="R34" s="26">
-        <f>R26</f>
-        <v>-0.89595687499999987</v>
-      </c>
-      <c r="S34" s="23"/>
-      <c r="T34" s="23"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="22">
+        <f>(Q24*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V35:AD35))</f>
+        <v>-0.40868665600000004</v>
+      </c>
+      <c r="R34" s="22"/>
+      <c r="S34" s="22"/>
+      <c r="T34" s="22"/>
     </row>
     <row r="35" spans="1:30">
-      <c r="U35" s="24" t="s">
+      <c r="U35" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="V35" s="25"/>
-      <c r="W35" s="27">
-        <f>W27</f>
-        <v>0.94762499999999994</v>
-      </c>
-      <c r="X35" s="25">
-        <f>(X33*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V37:AD37))-((1-LR0)*DISR*MAX(L36:T36))</f>
-        <v>1.7584477244531249</v>
-      </c>
-      <c r="Y35" s="25"/>
-      <c r="Z35" s="25"/>
-      <c r="AA35" s="25"/>
-      <c r="AB35" s="25"/>
-      <c r="AC35" s="25"/>
-      <c r="AD35" s="25"/>
+      <c r="V35" s="28"/>
+      <c r="W35" s="28"/>
+      <c r="X35" s="28">
+        <f>(X25*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L36:T36))</f>
+        <v>0.51140704000000003</v>
+      </c>
+      <c r="Y35" s="28"/>
+      <c r="Z35" s="28"/>
+      <c r="AA35" s="28"/>
+      <c r="AB35" s="28"/>
+      <c r="AC35" s="28"/>
+      <c r="AD35" s="28"/>
     </row>
     <row r="36" spans="1:30">
-      <c r="K36" s="13" t="s">
+      <c r="K36" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23"/>
-      <c r="N36" s="23"/>
-      <c r="O36" s="23"/>
-      <c r="P36" s="23"/>
-      <c r="Q36" s="23"/>
-      <c r="R36" s="23">
-        <f>(R34*LR0)+((1-LR0)*PLAY)+(0)-((1-LR0)*DISR*MAX(V37:AD37))</f>
-        <v>-0.90206567187499997</v>
-      </c>
-      <c r="S36" s="23"/>
-      <c r="T36" s="23"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="22"/>
+      <c r="P36" s="22"/>
+      <c r="Q36" s="22"/>
+      <c r="R36" s="22">
+        <f>(R26*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V37:AD37))</f>
+        <v>-0.63969200000000004</v>
+      </c>
+      <c r="S36" s="22"/>
+      <c r="T36" s="22"/>
     </row>
     <row r="37" spans="1:30">
-      <c r="U37" s="24" t="s">
+      <c r="U37" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="V37" s="25"/>
-      <c r="W37" s="25">
-        <f>(W35*LR0)+((1-LR0)*DISR*WIN)</f>
-        <v>0.94988125000000001</v>
-      </c>
-      <c r="X37" s="25"/>
-      <c r="Y37" s="25"/>
-      <c r="Z37" s="25"/>
-      <c r="AA37" s="25"/>
-      <c r="AB37" s="25"/>
-      <c r="AC37" s="25"/>
-      <c r="AD37" s="25"/>
+      <c r="V37" s="28"/>
+      <c r="W37" s="28">
+        <f>(W27*LR0)+((1-LR0)*DISR*WIN)</f>
+        <v>0.79990000000000006</v>
+      </c>
+      <c r="X37" s="28"/>
+      <c r="Y37" s="28"/>
+      <c r="Z37" s="28"/>
+      <c r="AA37" s="28"/>
+      <c r="AB37" s="28"/>
+      <c r="AC37" s="28"/>
+      <c r="AD37" s="28"/>
     </row>
     <row r="40" spans="1:30">
-      <c r="K40" s="13" t="s">
+      <c r="K40" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L40" s="23"/>
-      <c r="M40" s="23"/>
-      <c r="N40" s="23"/>
-      <c r="O40" s="23"/>
-      <c r="P40" s="23"/>
-      <c r="Q40" s="23"/>
-      <c r="R40" s="23"/>
-      <c r="S40" s="26">
-        <f>S32</f>
-        <v>-3.2428717286147255</v>
-      </c>
-      <c r="T40" s="23"/>
+      <c r="L40" s="22"/>
+      <c r="M40" s="22"/>
+      <c r="N40" s="22"/>
+      <c r="O40" s="22"/>
+      <c r="P40" s="22"/>
+      <c r="Q40" s="22"/>
+      <c r="R40" s="22"/>
+      <c r="S40" s="22"/>
+      <c r="T40" s="22"/>
     </row>
     <row r="41" spans="1:30">
-      <c r="U41" s="24" t="s">
+      <c r="U41" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="V41" s="27">
-        <f>V33</f>
-        <v>2.5192416996305176</v>
-      </c>
-      <c r="W41" s="25"/>
-      <c r="X41" s="25"/>
-      <c r="Y41" s="25"/>
-      <c r="Z41" s="25"/>
-      <c r="AA41" s="25"/>
-      <c r="AB41" s="25"/>
-      <c r="AC41" s="25"/>
-      <c r="AD41" s="25"/>
+      <c r="V41" s="28"/>
+      <c r="W41" s="28"/>
+      <c r="X41" s="28"/>
+      <c r="Y41" s="28"/>
+      <c r="Z41" s="28"/>
+      <c r="AA41" s="28"/>
+      <c r="AB41" s="28"/>
+      <c r="AC41" s="28"/>
+      <c r="AD41" s="28"/>
     </row>
     <row r="42" spans="1:30">
-      <c r="K42" s="13" t="s">
+      <c r="K42" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="L42" s="23"/>
-      <c r="M42" s="23"/>
-      <c r="N42" s="23"/>
-      <c r="O42" s="23"/>
-      <c r="P42" s="23"/>
-      <c r="Q42" s="26">
-        <f>Q34</f>
-        <v>-2.5254541334853515</v>
-      </c>
-      <c r="R42" s="23"/>
-      <c r="S42" s="23">
-        <f>(S40*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L44:T44))-((1-LR0)*DISR*MAX(V43:AD43))</f>
-        <v>-3.2580235579014278</v>
-      </c>
-      <c r="T42" s="23"/>
+      <c r="L42" s="22"/>
+      <c r="M42" s="22"/>
+      <c r="N42" s="22"/>
+      <c r="O42" s="22"/>
+      <c r="P42" s="22"/>
+      <c r="Q42" s="22"/>
+      <c r="R42" s="22"/>
+      <c r="S42" s="22">
+        <f>(S32*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V43:AD43))</f>
+        <v>-0.26197555289907204</v>
+      </c>
+      <c r="T42" s="22"/>
     </row>
     <row r="43" spans="1:30">
-      <c r="U43" s="24" t="s">
+      <c r="U43" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="V43" s="25">
-        <f>(V41*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V45:AD45))-((1-LR0)*DISR*MAX(L44:T44))</f>
-        <v>2.5282722466520822</v>
-      </c>
-      <c r="W43" s="25"/>
-      <c r="X43" s="27">
-        <f>X35</f>
-        <v>1.7584477244531249</v>
-      </c>
-      <c r="Y43" s="25"/>
-      <c r="Z43" s="25"/>
-      <c r="AA43" s="25"/>
-      <c r="AB43" s="25"/>
-      <c r="AC43" s="25"/>
-      <c r="AD43" s="25"/>
+      <c r="V43" s="28">
+        <f>(V33*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L44:T44))</f>
+        <v>0.32755818451200003</v>
+      </c>
+      <c r="W43" s="28"/>
+      <c r="X43" s="28"/>
+      <c r="Y43" s="28"/>
+      <c r="Z43" s="28"/>
+      <c r="AA43" s="28"/>
+      <c r="AB43" s="28"/>
+      <c r="AC43" s="28"/>
+      <c r="AD43" s="28"/>
     </row>
     <row r="44" spans="1:30">
-      <c r="K44" s="13" t="s">
+      <c r="K44" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="L44" s="23"/>
-      <c r="M44" s="23"/>
-      <c r="N44" s="23"/>
-      <c r="O44" s="23"/>
-      <c r="P44" s="23"/>
-      <c r="Q44" s="23">
-        <f>(Q42*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(L46:T46))-((1-LR0)*DISR*MAX(V45:AD45))</f>
-        <v>-2.5289504142901365</v>
-      </c>
-      <c r="R44" s="26">
-        <f>R36</f>
-        <v>-0.90206567187499997</v>
-      </c>
-      <c r="S44" s="23"/>
-      <c r="T44" s="23"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="22"/>
+      <c r="N44" s="22"/>
+      <c r="O44" s="22"/>
+      <c r="P44" s="22"/>
+      <c r="Q44" s="22">
+        <f>(Q34*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V45:AD45))</f>
+        <v>-0.40952071039999999</v>
+      </c>
+      <c r="R44" s="22"/>
+      <c r="S44" s="22"/>
+      <c r="T44" s="22"/>
     </row>
     <row r="45" spans="1:30">
-      <c r="U45" s="24" t="s">
+      <c r="U45" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="V45" s="25"/>
-      <c r="W45" s="27">
-        <f>W37</f>
-        <v>0.94988125000000001</v>
-      </c>
-      <c r="X45" s="25">
-        <f>(X43*LR0)+((1-LR0)*PLAY)+((1-LR0)*DISR*MAX(V47:AD47))-((1-LR0)*DISR*MAX(L46:T46))</f>
-        <v>1.759773842441406</v>
-      </c>
-      <c r="Y45" s="25"/>
-      <c r="Z45" s="25"/>
-      <c r="AA45" s="25"/>
-      <c r="AB45" s="25"/>
-      <c r="AC45" s="25"/>
-      <c r="AD45" s="25"/>
+      <c r="V45" s="28"/>
+      <c r="W45" s="28"/>
+      <c r="X45" s="28">
+        <f>(X35*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L46:T46))</f>
+        <v>0.51195575999999998</v>
+      </c>
+      <c r="Y45" s="28"/>
+      <c r="Z45" s="28"/>
+      <c r="AA45" s="28"/>
+      <c r="AB45" s="28"/>
+      <c r="AC45" s="28"/>
+      <c r="AD45" s="28"/>
     </row>
     <row r="46" spans="1:30">
-      <c r="K46" s="13" t="s">
+      <c r="K46" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="L46" s="23"/>
-      <c r="M46" s="23"/>
-      <c r="N46" s="23"/>
-      <c r="O46" s="23"/>
-      <c r="P46" s="23"/>
-      <c r="Q46" s="23"/>
-      <c r="R46" s="23">
-        <f>(R44*LR0)+((1-LR0)*PLAY)+(0)-((1-LR0)*DISR*MAX(V47:AD47))</f>
-        <v>-0.90247292499999998</v>
-      </c>
-      <c r="S46" s="23"/>
-      <c r="T46" s="23"/>
+      <c r="L46" s="22"/>
+      <c r="M46" s="22"/>
+      <c r="N46" s="22"/>
+      <c r="O46" s="22"/>
+      <c r="P46" s="22"/>
+      <c r="Q46" s="22"/>
+      <c r="R46" s="22">
+        <f>(R36*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V47:AD47))</f>
+        <v>-0.63998080000000002</v>
+      </c>
+      <c r="S46" s="22"/>
+      <c r="T46" s="22"/>
     </row>
     <row r="47" spans="1:30">
-      <c r="U47" s="24" t="s">
+      <c r="U47" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="V47" s="25"/>
-      <c r="W47" s="25">
-        <f>(W45*LR0)+((1-LR0)*DISR*WIN)</f>
-        <v>0.94999406249999996</v>
-      </c>
-      <c r="X47" s="25"/>
-      <c r="Y47" s="25"/>
-      <c r="Z47" s="25"/>
-      <c r="AA47" s="25"/>
-      <c r="AB47" s="25"/>
-      <c r="AC47" s="25"/>
-      <c r="AD47" s="25"/>
+      <c r="V47" s="28"/>
+      <c r="W47" s="28">
+        <f>(W37*LR0)+((1-LR0)*DISR*WIN)</f>
+        <v>0.79999500000000001</v>
+      </c>
+      <c r="X47" s="28"/>
+      <c r="Y47" s="28"/>
+      <c r="Z47" s="28"/>
+      <c r="AA47" s="28"/>
+      <c r="AB47" s="28"/>
+      <c r="AC47" s="28"/>
+      <c r="AD47" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1690,101 +1633,101 @@
     <col min="18" max="20" width="4" customWidth="1"/>
     <col min="21" max="21" width="5.42578125" customWidth="1"/>
     <col min="22" max="22" width="28.85546875" customWidth="1"/>
-    <col min="23" max="23" width="5.42578125" style="16" customWidth="1"/>
+    <col min="23" max="23" width="5.42578125" style="15" customWidth="1"/>
     <col min="24" max="24" width="7.140625" customWidth="1"/>
-    <col min="25" max="33" width="6.85546875" style="16" customWidth="1"/>
+    <col min="25" max="33" width="6.85546875" style="15" customWidth="1"/>
     <col min="34" max="34" width="7.42578125" customWidth="1"/>
-    <col min="35" max="43" width="6.85546875" style="16" customWidth="1"/>
+    <col min="35" max="43" width="6.85546875" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="15.75" thickBot="1">
-      <c r="Y1" s="19" t="s">
+      <c r="Y1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="14"/>
-      <c r="AI1" s="19" t="s">
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
+      <c r="AB1" s="18"/>
+      <c r="AC1" s="18"/>
+      <c r="AD1" s="18"/>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="13"/>
+      <c r="AI1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="AJ1" s="19"/>
-      <c r="AK1" s="19"/>
-      <c r="AL1" s="19"/>
-      <c r="AM1" s="19"/>
-      <c r="AN1" s="19"/>
-      <c r="AO1" s="19"/>
-      <c r="AP1" s="19"/>
-      <c r="AQ1" s="20"/>
+      <c r="AJ1" s="18"/>
+      <c r="AK1" s="18"/>
+      <c r="AL1" s="18"/>
+      <c r="AM1" s="18"/>
+      <c r="AN1" s="18"/>
+      <c r="AO1" s="18"/>
+      <c r="AP1" s="18"/>
+      <c r="AQ1" s="19"/>
     </row>
     <row r="2" spans="1:43">
       <c r="C2" s="4"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
-      <c r="V2" s="17" t="s">
+      <c r="V2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="W2" s="18">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="15">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="15">
+      <c r="W2" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="14">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="14">
         <v>2</v>
       </c>
-      <c r="AA2" s="15">
+      <c r="AA2" s="14">
         <v>3</v>
       </c>
-      <c r="AB2" s="15">
+      <c r="AB2" s="14">
         <v>4</v>
       </c>
-      <c r="AC2" s="15">
+      <c r="AC2" s="14">
         <v>5</v>
       </c>
-      <c r="AD2" s="15">
+      <c r="AD2" s="14">
         <v>6</v>
       </c>
-      <c r="AE2" s="15">
+      <c r="AE2" s="14">
         <v>7</v>
       </c>
-      <c r="AF2" s="15">
+      <c r="AF2" s="14">
         <v>8</v>
       </c>
-      <c r="AG2" s="15">
+      <c r="AG2" s="14">
         <v>9</v>
       </c>
-      <c r="AH2" s="14"/>
-      <c r="AI2" s="15">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="15">
+      <c r="AH2" s="13"/>
+      <c r="AI2" s="14">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="14">
         <v>2</v>
       </c>
-      <c r="AK2" s="15">
+      <c r="AK2" s="14">
         <v>3</v>
       </c>
-      <c r="AL2" s="15">
+      <c r="AL2" s="14">
         <v>4</v>
       </c>
-      <c r="AM2" s="15">
+      <c r="AM2" s="14">
         <v>5</v>
       </c>
-      <c r="AN2" s="15">
+      <c r="AN2" s="14">
         <v>6</v>
       </c>
-      <c r="AO2" s="15">
+      <c r="AO2" s="14">
         <v>7</v>
       </c>
-      <c r="AP2" s="15">
+      <c r="AP2" s="14">
         <v>8</v>
       </c>
-      <c r="AQ2" s="15">
+      <c r="AQ2" s="14">
         <v>9</v>
       </c>
     </row>
@@ -1798,64 +1741,64 @@
       <c r="G3" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="17" t="s">
+      <c r="V3" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="W3" s="18">
+      <c r="W3" s="17">
         <v>5</v>
       </c>
-      <c r="Y3" s="16">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="16">
+      <c r="Y3" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="15">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="15">
         <v>0</v>
       </c>
     </row>
@@ -1863,34 +1806,34 @@
       <c r="C4" s="10"/>
       <c r="D4" s="11"/>
       <c r="E4" s="12"/>
-      <c r="V4" s="17" t="s">
+      <c r="V4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="W4" s="18">
+      <c r="W4" s="17">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:43">
-      <c r="V5" s="17"/>
-      <c r="W5" s="18"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="17"/>
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1">
-      <c r="V6" s="17" t="s">
+      <c r="V6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="W6" s="18">
+      <c r="W6" s="17">
         <v>0.05</v>
       </c>
-      <c r="X6" s="16"/>
+      <c r="X6" s="15"/>
     </row>
     <row r="7" spans="1:43">
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
-      <c r="V7" s="17" t="s">
+      <c r="V7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="W7" s="18">
+      <c r="W7" s="17">
         <v>0.1</v>
       </c>
     </row>
@@ -1904,10 +1847,10 @@
       <c r="G8" t="s">
         <v>11</v>
       </c>
-      <c r="V8" s="17" t="s">
+      <c r="V8" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="W8" s="18">
+      <c r="W8" s="17">
         <v>0.95</v>
       </c>
     </row>
@@ -1927,43 +1870,43 @@
       <c r="X10" t="s">
         <v>12</v>
       </c>
-      <c r="Y10" s="16">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="16">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="16">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="16">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="16">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="16">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="16">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="21">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="16">
+      <c r="Y10" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="15">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:43" ht="15.75" thickBot="1">
       <c r="A11" s="2"/>
-      <c r="V11" s="17" t="s">
+      <c r="V11" s="16" t="s">
         <v>16</v>
       </c>
       <c r="X11" t="s">
         <v>11</v>
       </c>
-      <c r="AF11" s="16">
+      <c r="AF11" s="15">
         <f>(AF10*LR0)+((1-LR0)*PLAY)+((1-LR0)*MAX(Y12:AG12))</f>
         <v>0.95</v>
       </c>
@@ -1975,7 +1918,7 @@
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
-      <c r="V12" s="17" t="s">
+      <c r="V12" s="16" t="s">
         <v>17</v>
       </c>
       <c r="X12" t="s">
@@ -1992,7 +1935,7 @@
       <c r="G13" t="s">
         <v>19</v>
       </c>
-      <c r="V13" s="17" t="s">
+      <c r="V13" s="16" t="s">
         <v>18</v>
       </c>
       <c r="X13" t="s">

</xml_diff>

<commit_message>
More work on the q vals; still needs a big clean-up and refeactor
</commit_message>
<xml_diff>
--- a/UseCase816372.xlsx
+++ b/UseCase816372.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="23955" windowHeight="14130"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="23955" windowHeight="14130" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="816372UseCase" sheetId="1" r:id="rId1"/>
     <sheet name="816372UseCase (2)" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="DISR" localSheetId="1">'816372UseCase (2)'!$W$8</definedName>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="28">
   <si>
     <t>X</t>
   </si>
@@ -53,6 +54,9 @@
   </si>
   <si>
     <t>Q Vals for Actions (O)</t>
+  </si>
+  <si>
+    <t>LR0</t>
   </si>
   <si>
     <t>LR Decay</t>
@@ -105,6 +109,12 @@
   <si>
     <t>s0(O)</t>
   </si>
+  <si>
+    <t>LRD</t>
+  </si>
+  <si>
+    <t>MITR</t>
+  </si>
 </sst>
 </file>
 
@@ -113,7 +123,14 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,18 +335,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -359,35 +377,416 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$I$3:$I$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>4.9900199600798403E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.566333808844508E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.774694783573807E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2706630336058131E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.921598770176787E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6655562958027982E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4697236919459141E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.315097317201473E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1899095668729178E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0864841373315949E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.9960015993602568E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.2558311736393936E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.617718028266115E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.0619155111254434E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.5734625870948202E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7.1408169094544418E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.754931099702783E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6.4086131761086898E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.0960741282613997E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.8126017205301092E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.5543212619417904E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.318017443097213E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.100999795960009E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.9009998039600084E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.7160913035276366E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.5446282494091984E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.3851955797228554E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.2365700728690054E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="75468800"/>
+        <c:axId val="75470720"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="75468800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75470720"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="75470720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="75468800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$J$3:$J$30</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0.95009980039920161</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96433666191155487</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97225305216426194</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97729336966394187</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98078401229823209</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.98334443704197205</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.98530276308054088</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.98684902682798525</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.98810090433127085</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.989135158626684</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9900039984006398</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.99074416882636063</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.99138228197173384</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.99193808448887455</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99242653741290521</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99285918309054555</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.99324506890029718</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99359138682389136</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.99390392587173859</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99418739827946989</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.99444567873805823</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99468198255690277</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99489900020403998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.99509900019604003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.99528390869647232</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.99545537175059085</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.99561480442027717</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.99576342992713096</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="79031296"/>
+        <c:axId val="80966784"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="79031296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="80966784"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="80966784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="79031296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -677,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AD47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="W47" sqref="W47"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -796,7 +1195,7 @@
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I3" s="16" t="s">
         <v>4</v>
@@ -876,7 +1275,7 @@
     </row>
     <row r="6" spans="1:30" ht="15.75" thickBot="1">
       <c r="I6" s="16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J6" s="17">
         <v>0.05</v>
@@ -887,7 +1286,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
       <c r="I7" s="16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J7" s="17">
         <v>0.1</v>
@@ -901,13 +1300,13 @@
       <c r="D8" s="8"/>
       <c r="E8" s="9"/>
       <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="16" t="s">
-        <v>10</v>
-      </c>
       <c r="J8" s="17">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="15.75" thickBot="1">
@@ -921,10 +1320,10 @@
     <row r="10" spans="1:30">
       <c r="A10" s="2"/>
       <c r="I10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L10" s="22"/>
       <c r="M10" s="22"/>
@@ -939,10 +1338,10 @@
     <row r="11" spans="1:30" ht="15.75" thickBot="1">
       <c r="A11" s="2"/>
       <c r="I11" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="U11" s="28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="V11" s="28"/>
       <c r="W11" s="28"/>
@@ -962,10 +1361,10 @@
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
       <c r="I12" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="22"/>
@@ -976,7 +1375,7 @@
       <c r="R12" s="22"/>
       <c r="S12" s="22">
         <f>(S10*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V13:AD13))</f>
-        <v>-0.19269992857600002</v>
+        <v>-0.54036008766263688</v>
       </c>
       <c r="T12" s="22"/>
     </row>
@@ -988,17 +1387,17 @@
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
       <c r="G13" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="16" t="s">
-        <v>18</v>
-      </c>
       <c r="U13" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V13" s="28">
         <f>(V11*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L14:T14))</f>
-        <v>0.25355253760000002</v>
+        <v>0.59873693923837878</v>
       </c>
       <c r="W13" s="28"/>
       <c r="X13" s="28"/>
@@ -1017,7 +1416,7 @@
       </c>
       <c r="E14" s="12"/>
       <c r="K14" s="22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L14" s="22"/>
       <c r="M14" s="22"/>
@@ -1026,7 +1425,7 @@
       <c r="P14" s="22"/>
       <c r="Q14" s="22">
         <f>(Q12*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V15:AD15))</f>
-        <v>-0.33362176000000004</v>
+        <v>-0.66342043128906236</v>
       </c>
       <c r="R14" s="22"/>
       <c r="S14" s="22"/>
@@ -1035,13 +1434,13 @@
     <row r="15" spans="1:30">
       <c r="A15" s="2"/>
       <c r="U15" s="28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V15" s="28"/>
       <c r="W15" s="28"/>
       <c r="X15" s="28">
         <f>(X13*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L16:T16))</f>
-        <v>0.43897600000000003</v>
+        <v>0.73509189062499991</v>
       </c>
       <c r="Y15" s="28"/>
       <c r="Z15" s="28"/>
@@ -1053,7 +1452,7 @@
     <row r="16" spans="1:30" ht="15.75" thickBot="1">
       <c r="A16" s="2"/>
       <c r="K16" s="22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
@@ -1063,7 +1462,7 @@
       <c r="Q16" s="22"/>
       <c r="R16" s="22">
         <f>(R14*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V17:AD17))</f>
-        <v>-0.5776</v>
+        <v>-0.81450624999999999</v>
       </c>
       <c r="S16" s="22"/>
       <c r="T16" s="22"/>
@@ -1076,12 +1475,12 @@
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
       <c r="U17" s="28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="V17" s="28"/>
       <c r="W17" s="28">
         <f>(W15*LR0)+((1-LR0)*DISR*WIN)</f>
-        <v>0.76</v>
+        <v>0.90249999999999997</v>
       </c>
       <c r="X17" s="28"/>
       <c r="Y17" s="28"/>
@@ -1101,7 +1500,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="15.75" thickBot="1">
@@ -1115,7 +1514,7 @@
     <row r="20" spans="1:30">
       <c r="A20" s="2"/>
       <c r="K20" s="22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L20" s="22"/>
       <c r="M20" s="22"/>
@@ -1130,7 +1529,7 @@
     <row r="21" spans="1:30" ht="15.75" thickBot="1">
       <c r="A21" s="2"/>
       <c r="U21" s="28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="V21" s="28"/>
       <c r="W21" s="28"/>
@@ -1152,7 +1551,7 @@
         <v>1</v>
       </c>
       <c r="K22" s="22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L22" s="22"/>
       <c r="M22" s="22"/>
@@ -1163,7 +1562,7 @@
       <c r="R22" s="22"/>
       <c r="S22" s="22">
         <f>(S12*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V23:AD23))</f>
-        <v>-0.25050990714880006</v>
+        <v>-0.70246811396142783</v>
       </c>
       <c r="T22" s="22"/>
     </row>
@@ -1177,14 +1576,14 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U23" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V23" s="28">
         <f>(V13*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L24:T24))</f>
-        <v>0.31694067200000003</v>
+        <v>0.74842117404797337</v>
       </c>
       <c r="W23" s="28"/>
       <c r="X23" s="28"/>
@@ -1203,7 +1602,7 @@
       </c>
       <c r="E24" s="12"/>
       <c r="K24" s="22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L24" s="22"/>
       <c r="M24" s="22"/>
@@ -1212,7 +1611,7 @@
       <c r="P24" s="22"/>
       <c r="Q24" s="22">
         <f>(Q14*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V25:AD25))</f>
-        <v>-0.40034611200000003</v>
+        <v>-0.79610451754687483</v>
       </c>
       <c r="R24" s="22"/>
       <c r="S24" s="22"/>
@@ -1221,13 +1620,13 @@
     <row r="25" spans="1:30">
       <c r="A25" s="2"/>
       <c r="U25" s="28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V25" s="28"/>
       <c r="W25" s="28"/>
       <c r="X25" s="28">
         <f>(X15*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L26:T26))</f>
-        <v>0.5048224</v>
+        <v>0.8453556742187498</v>
       </c>
       <c r="Y25" s="28"/>
       <c r="Z25" s="28"/>
@@ -1239,7 +1638,7 @@
     <row r="26" spans="1:30" ht="15.75" thickBot="1">
       <c r="A26" s="2"/>
       <c r="K26" s="22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L26" s="22"/>
       <c r="M26" s="22"/>
@@ -1249,7 +1648,7 @@
       <c r="Q26" s="22"/>
       <c r="R26" s="22">
         <f>(R16*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V27:AD27))</f>
-        <v>-0.63536000000000004</v>
+        <v>-0.89595687499999987</v>
       </c>
       <c r="S26" s="22"/>
       <c r="T26" s="22"/>
@@ -1264,12 +1663,12 @@
         <v>1</v>
       </c>
       <c r="U27" s="28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="V27" s="28"/>
       <c r="W27" s="28">
         <f>(W17*LR0)+((1-LR0)*DISR*WIN)</f>
-        <v>0.79800000000000004</v>
+        <v>0.94762499999999994</v>
       </c>
       <c r="X27" s="28"/>
       <c r="Y27" s="28"/>
@@ -1289,10 +1688,10 @@
         <v>0</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:30" ht="15.75" thickBot="1">
@@ -1308,7 +1707,7 @@
     <row r="30" spans="1:30">
       <c r="A30" s="2"/>
       <c r="K30" s="22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L30" s="22"/>
       <c r="M30" s="22"/>
@@ -1323,7 +1722,7 @@
     <row r="31" spans="1:30" ht="15.75" thickBot="1">
       <c r="A31" s="2"/>
       <c r="U31" s="28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="V31" s="28"/>
       <c r="W31" s="28"/>
@@ -1347,7 +1746,7 @@
         <v>1</v>
       </c>
       <c r="K32" s="22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
@@ -1358,7 +1757,7 @@
       <c r="R32" s="22"/>
       <c r="S32" s="22">
         <f>(S22*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V33:AD33))</f>
-        <v>-0.26062665339904006</v>
+        <v>-0.73083701856371619</v>
       </c>
       <c r="T32" s="22"/>
     </row>
@@ -1372,17 +1771,17 @@
         <v>0</v>
       </c>
       <c r="G33" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H33" t="s">
         <v>4</v>
       </c>
       <c r="U33" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V33" s="28">
         <f>(V23*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L34:T34))</f>
-        <v>0.32644889216000006</v>
+        <v>0.77087380926941262</v>
       </c>
       <c r="W33" s="28"/>
       <c r="X33" s="28"/>
@@ -1402,7 +1801,7 @@
       </c>
       <c r="E34" s="12"/>
       <c r="K34" s="22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L34" s="22"/>
       <c r="M34" s="22"/>
@@ -1411,7 +1810,7 @@
       <c r="P34" s="22"/>
       <c r="Q34" s="22">
         <f>(Q24*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V35:AD35))</f>
-        <v>-0.40868665600000004</v>
+        <v>-0.81269002832910142</v>
       </c>
       <c r="R34" s="22"/>
       <c r="S34" s="22"/>
@@ -1419,13 +1818,13 @@
     </row>
     <row r="35" spans="1:30">
       <c r="U35" s="28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V35" s="28"/>
       <c r="W35" s="28"/>
       <c r="X35" s="28">
         <f>(X25*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L36:T36))</f>
-        <v>0.51140704000000003</v>
+        <v>0.85638205257812494</v>
       </c>
       <c r="Y35" s="28"/>
       <c r="Z35" s="28"/>
@@ -1436,7 +1835,7 @@
     </row>
     <row r="36" spans="1:30">
       <c r="K36" s="22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L36" s="22"/>
       <c r="M36" s="22"/>
@@ -1446,19 +1845,19 @@
       <c r="Q36" s="22"/>
       <c r="R36" s="22">
         <f>(R26*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V37:AD37))</f>
-        <v>-0.63969200000000004</v>
+        <v>-0.90206567187499997</v>
       </c>
       <c r="S36" s="22"/>
       <c r="T36" s="22"/>
     </row>
     <row r="37" spans="1:30">
       <c r="U37" s="28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="V37" s="28"/>
       <c r="W37" s="28">
         <f>(W27*LR0)+((1-LR0)*DISR*WIN)</f>
-        <v>0.79990000000000006</v>
+        <v>0.94988125000000001</v>
       </c>
       <c r="X37" s="28"/>
       <c r="Y37" s="28"/>
@@ -1470,7 +1869,7 @@
     </row>
     <row r="40" spans="1:30">
       <c r="K40" s="22" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L40" s="22"/>
       <c r="M40" s="22"/>
@@ -1484,7 +1883,7 @@
     </row>
     <row r="41" spans="1:30">
       <c r="U41" s="28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="V41" s="28"/>
       <c r="W41" s="28"/>
@@ -1498,7 +1897,7 @@
     </row>
     <row r="42" spans="1:30">
       <c r="K42" s="22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L42" s="22"/>
       <c r="M42" s="22"/>
@@ -1509,17 +1908,17 @@
       <c r="R42" s="22"/>
       <c r="S42" s="22">
         <f>(S32*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V43:AD43))</f>
-        <v>-0.26197555289907204</v>
+        <v>-0.73461953917735479</v>
       </c>
       <c r="T42" s="22"/>
     </row>
     <row r="43" spans="1:30">
       <c r="U43" s="28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V43" s="28">
         <f>(V33*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L44:T44))</f>
-        <v>0.32755818451200003</v>
+        <v>0.77349328337858059</v>
       </c>
       <c r="W43" s="28"/>
       <c r="X43" s="28"/>
@@ -1532,7 +1931,7 @@
     </row>
     <row r="44" spans="1:30">
       <c r="K44" s="22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="L44" s="22"/>
       <c r="M44" s="22"/>
@@ -1541,7 +1940,7 @@
       <c r="P44" s="22"/>
       <c r="Q44" s="22">
         <f>(Q34*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V45:AD45))</f>
-        <v>-0.40952071039999999</v>
+        <v>-0.81434857940732408</v>
       </c>
       <c r="R44" s="22"/>
       <c r="S44" s="22"/>
@@ -1549,13 +1948,13 @@
     </row>
     <row r="45" spans="1:30">
       <c r="U45" s="28" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="V45" s="28"/>
       <c r="W45" s="28"/>
       <c r="X45" s="28">
         <f>(X35*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(L46:T46))</f>
-        <v>0.51195575999999998</v>
+        <v>0.85730091744140613</v>
       </c>
       <c r="Y45" s="28"/>
       <c r="Z45" s="28"/>
@@ -1566,7 +1965,7 @@
     </row>
     <row r="46" spans="1:30">
       <c r="K46" s="22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L46" s="22"/>
       <c r="M46" s="22"/>
@@ -1576,19 +1975,19 @@
       <c r="Q46" s="22"/>
       <c r="R46" s="22">
         <f>(R36*LR0)+((1-LR0)*PLAY)-((1-LR0)*DISR*MAX(V47:AD47))</f>
-        <v>-0.63998080000000002</v>
+        <v>-0.90247292499999998</v>
       </c>
       <c r="S46" s="22"/>
       <c r="T46" s="22"/>
     </row>
     <row r="47" spans="1:30">
       <c r="U47" s="28" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="V47" s="28"/>
       <c r="W47" s="28">
         <f>(W37*LR0)+((1-LR0)*DISR*WIN)</f>
-        <v>0.79999500000000001</v>
+        <v>0.94999406249999996</v>
       </c>
       <c r="X47" s="28"/>
       <c r="Y47" s="28"/>
@@ -1739,7 +2138,7 @@
       <c r="D3" s="8"/>
       <c r="E3" s="9"/>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="V3" s="16" t="s">
         <v>4</v>
@@ -1819,7 +2218,7 @@
     </row>
     <row r="6" spans="1:43" ht="15.75" thickBot="1">
       <c r="V6" s="16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="W6" s="17">
         <v>0.05</v>
@@ -1831,7 +2230,7 @@
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
       <c r="V7" s="16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="W7" s="17">
         <v>0.1</v>
@@ -1845,10 +2244,10 @@
       <c r="D8" s="8"/>
       <c r="E8" s="9"/>
       <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="V8" s="16" t="s">
         <v>11</v>
-      </c>
-      <c r="V8" s="16" t="s">
-        <v>10</v>
       </c>
       <c r="W8" s="17">
         <v>0.95</v>
@@ -1865,10 +2264,10 @@
     <row r="10" spans="1:43">
       <c r="A10" s="2"/>
       <c r="V10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="X10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Y10" s="15">
         <v>0</v>
@@ -1901,10 +2300,10 @@
     <row r="11" spans="1:43" ht="15.75" thickBot="1">
       <c r="A11" s="2"/>
       <c r="V11" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="X11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AF11" s="15">
         <f>(AF10*LR0)+((1-LR0)*PLAY)+((1-LR0)*MAX(Y12:AG12))</f>
@@ -1919,10 +2318,10 @@
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
       <c r="V12" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="X12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:43">
@@ -1933,13 +2332,13 @@
       <c r="D13" s="8"/>
       <c r="E13" s="9"/>
       <c r="G13" t="s">
+        <v>20</v>
+      </c>
+      <c r="V13" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="V13" s="16" t="s">
-        <v>18</v>
-      </c>
       <c r="X13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:43" ht="15.75" thickBot="1">
@@ -1974,7 +2373,7 @@
         <v>0</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="15.75" thickBot="1">
@@ -2011,7 +2410,7 @@
         <v>0</v>
       </c>
       <c r="G23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="15.75" thickBot="1">
@@ -2244,4 +2643,545 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="C3:J30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="9" max="9" width="9.140625" style="30"/>
+    <col min="10" max="10" width="9.140625" style="29"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:10">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>0.05</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <f>1+G3*$D$4</f>
+        <v>1.002</v>
+      </c>
+      <c r="I3" s="30">
+        <f>$D$3/H3</f>
+        <v>4.9900199600798403E-2</v>
+      </c>
+      <c r="J3" s="29">
+        <f>1-I3</f>
+        <v>0.95009980039920161</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10">
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4">
+        <v>2E-3</v>
+      </c>
+      <c r="G4">
+        <f>G3+(6000/30)</f>
+        <v>201</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H30" si="0">1+G4*$D$4</f>
+        <v>1.4020000000000001</v>
+      </c>
+      <c r="I4" s="30">
+        <f t="shared" ref="I4:I30" si="1">$D$3/H4</f>
+        <v>3.566333808844508E-2</v>
+      </c>
+      <c r="J4" s="29">
+        <f t="shared" ref="J4:J30" si="2">1-I4</f>
+        <v>0.96433666191155487</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10">
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G30" si="3">G4+(6000/30)</f>
+        <v>401</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>1.802</v>
+      </c>
+      <c r="I5" s="30">
+        <f t="shared" si="1"/>
+        <v>2.774694783573807E-2</v>
+      </c>
+      <c r="J5" s="29">
+        <f t="shared" si="2"/>
+        <v>0.97225305216426194</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10">
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>601</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>2.202</v>
+      </c>
+      <c r="I6" s="30">
+        <f t="shared" si="1"/>
+        <v>2.2706630336058131E-2</v>
+      </c>
+      <c r="J6" s="29">
+        <f t="shared" si="2"/>
+        <v>0.97729336966394187</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10">
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>801</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>2.6020000000000003</v>
+      </c>
+      <c r="I7" s="30">
+        <f t="shared" si="1"/>
+        <v>1.921598770176787E-2</v>
+      </c>
+      <c r="J7" s="29">
+        <f t="shared" si="2"/>
+        <v>0.98078401229823209</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10">
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>1001</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>3.0020000000000002</v>
+      </c>
+      <c r="I8" s="30">
+        <f t="shared" si="1"/>
+        <v>1.6655562958027982E-2</v>
+      </c>
+      <c r="J8" s="29">
+        <f t="shared" si="2"/>
+        <v>0.98334443704197205</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10">
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>1201</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>3.4020000000000001</v>
+      </c>
+      <c r="I9" s="30">
+        <f t="shared" si="1"/>
+        <v>1.4697236919459141E-2</v>
+      </c>
+      <c r="J9" s="29">
+        <f t="shared" si="2"/>
+        <v>0.98530276308054088</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10">
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>1401</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>3.802</v>
+      </c>
+      <c r="I10" s="30">
+        <f t="shared" si="1"/>
+        <v>1.315097317201473E-2</v>
+      </c>
+      <c r="J10" s="29">
+        <f t="shared" si="2"/>
+        <v>0.98684902682798525</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10">
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>1601</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>4.202</v>
+      </c>
+      <c r="I11" s="30">
+        <f t="shared" si="1"/>
+        <v>1.1899095668729178E-2</v>
+      </c>
+      <c r="J11" s="29">
+        <f t="shared" si="2"/>
+        <v>0.98810090433127085</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10">
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>1801</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>4.6020000000000003</v>
+      </c>
+      <c r="I12" s="30">
+        <f t="shared" si="1"/>
+        <v>1.0864841373315949E-2</v>
+      </c>
+      <c r="J12" s="29">
+        <f t="shared" si="2"/>
+        <v>0.989135158626684</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10">
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>2001</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>5.0019999999999998</v>
+      </c>
+      <c r="I13" s="30">
+        <f t="shared" si="1"/>
+        <v>9.9960015993602568E-3</v>
+      </c>
+      <c r="J13" s="29">
+        <f t="shared" si="2"/>
+        <v>0.9900039984006398</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10">
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>2201</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>5.4020000000000001</v>
+      </c>
+      <c r="I14" s="30">
+        <f t="shared" si="1"/>
+        <v>9.2558311736393936E-3</v>
+      </c>
+      <c r="J14" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99074416882636063</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10">
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>2401</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>5.8020000000000005</v>
+      </c>
+      <c r="I15" s="30">
+        <f t="shared" si="1"/>
+        <v>8.617718028266115E-3</v>
+      </c>
+      <c r="J15" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99138228197173384</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10">
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>2601</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>6.202</v>
+      </c>
+      <c r="I16" s="30">
+        <f t="shared" si="1"/>
+        <v>8.0619155111254434E-3</v>
+      </c>
+      <c r="J16" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99193808448887455</v>
+      </c>
+    </row>
+    <row r="17" spans="7:10">
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>2801</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>6.6020000000000003</v>
+      </c>
+      <c r="I17" s="30">
+        <f t="shared" si="1"/>
+        <v>7.5734625870948202E-3</v>
+      </c>
+      <c r="J17" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99242653741290521</v>
+      </c>
+    </row>
+    <row r="18" spans="7:10">
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>3001</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>7.0019999999999998</v>
+      </c>
+      <c r="I18" s="30">
+        <f t="shared" si="1"/>
+        <v>7.1408169094544418E-3</v>
+      </c>
+      <c r="J18" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99285918309054555</v>
+      </c>
+    </row>
+    <row r="19" spans="7:10">
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>3201</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>7.4020000000000001</v>
+      </c>
+      <c r="I19" s="30">
+        <f t="shared" si="1"/>
+        <v>6.754931099702783E-3</v>
+      </c>
+      <c r="J19" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99324506890029718</v>
+      </c>
+    </row>
+    <row r="20" spans="7:10">
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>3401</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>7.8020000000000005</v>
+      </c>
+      <c r="I20" s="30">
+        <f t="shared" si="1"/>
+        <v>6.4086131761086898E-3</v>
+      </c>
+      <c r="J20" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99359138682389136</v>
+      </c>
+    </row>
+    <row r="21" spans="7:10">
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>3601</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>8.202</v>
+      </c>
+      <c r="I21" s="30">
+        <f t="shared" si="1"/>
+        <v>6.0960741282613997E-3</v>
+      </c>
+      <c r="J21" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99390392587173859</v>
+      </c>
+    </row>
+    <row r="22" spans="7:10">
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>3801</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>8.6020000000000003</v>
+      </c>
+      <c r="I22" s="30">
+        <f t="shared" si="1"/>
+        <v>5.8126017205301092E-3</v>
+      </c>
+      <c r="J22" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99418739827946989</v>
+      </c>
+    </row>
+    <row r="23" spans="7:10">
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>4001</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>9.0020000000000007</v>
+      </c>
+      <c r="I23" s="30">
+        <f t="shared" si="1"/>
+        <v>5.5543212619417904E-3</v>
+      </c>
+      <c r="J23" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99444567873805823</v>
+      </c>
+    </row>
+    <row r="24" spans="7:10">
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>4201</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>9.402000000000001</v>
+      </c>
+      <c r="I24" s="30">
+        <f t="shared" si="1"/>
+        <v>5.318017443097213E-3</v>
+      </c>
+      <c r="J24" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99468198255690277</v>
+      </c>
+    </row>
+    <row r="25" spans="7:10">
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>4401</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>9.8019999999999996</v>
+      </c>
+      <c r="I25" s="30">
+        <f t="shared" si="1"/>
+        <v>5.100999795960009E-3</v>
+      </c>
+      <c r="J25" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99489900020403998</v>
+      </c>
+    </row>
+    <row r="26" spans="7:10">
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>4601</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>10.202</v>
+      </c>
+      <c r="I26" s="30">
+        <f t="shared" si="1"/>
+        <v>4.9009998039600084E-3</v>
+      </c>
+      <c r="J26" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99509900019604003</v>
+      </c>
+    </row>
+    <row r="27" spans="7:10">
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>4801</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>10.602</v>
+      </c>
+      <c r="I27" s="30">
+        <f t="shared" si="1"/>
+        <v>4.7160913035276366E-3</v>
+      </c>
+      <c r="J27" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99528390869647232</v>
+      </c>
+    </row>
+    <row r="28" spans="7:10">
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>5001</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>11.002000000000001</v>
+      </c>
+      <c r="I28" s="30">
+        <f t="shared" si="1"/>
+        <v>4.5446282494091984E-3</v>
+      </c>
+      <c r="J28" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99545537175059085</v>
+      </c>
+    </row>
+    <row r="29" spans="7:10">
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>5201</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>11.402000000000001</v>
+      </c>
+      <c r="I29" s="30">
+        <f t="shared" si="1"/>
+        <v>4.3851955797228554E-3</v>
+      </c>
+      <c r="J29" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99561480442027717</v>
+      </c>
+    </row>
+    <row r="30" spans="7:10">
+      <c r="G30">
+        <f t="shared" si="3"/>
+        <v>5401</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>11.802</v>
+      </c>
+      <c r="I30" s="30">
+        <f t="shared" si="1"/>
+        <v>4.2365700728690054E-3</v>
+      </c>
+      <c r="J30" s="29">
+        <f t="shared" si="2"/>
+        <v>0.99576342992713096</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>